<commit_message>
about to put in conclusion and discussion edits
</commit_message>
<xml_diff>
--- a/Report/childMetrics.xlsx
+++ b/Report/childMetrics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17000" tabRatio="500"/>
+    <workbookView xWindow="480" yWindow="0" windowWidth="25120" windowHeight="14180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -157,13 +157,13 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -526,7 +526,7 @@
   <dimension ref="A2:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:K6"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -537,64 +537,64 @@
   <sheetData>
     <row r="2" spans="1:11">
       <c r="A2" s="1"/>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="4"/>
       <c r="F2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G2" s="3"/>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2" t="s">
+      <c r="I2" s="4"/>
+      <c r="J2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="2"/>
+      <c r="K2" s="4"/>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="1">
@@ -629,7 +629,7 @@
       </c>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1">
@@ -664,7 +664,7 @@
       </c>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1">
@@ -692,7 +692,7 @@
         <v>0.87139999999999995</v>
       </c>
       <c r="J6" s="1">
-        <v>0.88570000000000004</v>
+        <v>0.75</v>
       </c>
       <c r="K6" s="1">
         <v>0.52939999999999998</v>

</xml_diff>